<commit_message>
Ajout du parser de forum
</commit_message>
<xml_diff>
--- a/excel/forum.xlsx
+++ b/excel/forum.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="430">
   <si>
     <t>LISTE DES ENTREPRISES PRESENTES AU FORUM DES ENTREPRISES 2016</t>
   </si>
@@ -1288,6 +1288,27 @@
   </si>
   <si>
     <t>27 RUE DES GRANGES GALAND</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>DI / DII</t>
+  </si>
+  <si>
+    <t>Bac+5</t>
+  </si>
+  <si>
+    <t>oi</t>
+  </si>
+  <si>
+    <t>DI STMG</t>
+  </si>
+  <si>
+    <t>BAC++</t>
+  </si>
+  <si>
+    <t>COMMENTAIRE</t>
   </si>
 </sst>
 </file>
@@ -1794,11 +1815,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
@@ -1932,7 +1970,9 @@
       <c r="H4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>423</v>
+      </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="6"/>
@@ -1966,7 +2006,9 @@
         <v>36</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="8"/>
+      <c r="J5" s="8" t="s">
+        <v>423</v>
+      </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
@@ -2006,7 +2048,9 @@
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="9"/>
+      <c r="K6" s="9" t="s">
+        <v>423</v>
+      </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
@@ -2046,7 +2090,9 @@
       <c r="I7" s="9"/>
       <c r="J7" s="8"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="L7" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="M7" s="9"/>
       <c r="N7" s="10"/>
       <c r="O7" s="6" t="s">
@@ -2086,7 +2132,9 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
+      <c r="M8" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="N8" s="10"/>
       <c r="O8" s="6" t="s">
         <v>61</v>
@@ -2126,7 +2174,9 @@
       <c r="K9" s="8"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
+      <c r="N9" s="10" t="s">
+        <v>423</v>
+      </c>
       <c r="O9" s="6" t="s">
         <v>70</v>
       </c>
@@ -2160,12 +2210,24 @@
       <c r="H10" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="10"/>
+      <c r="I10" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>429</v>
+      </c>
       <c r="O10" s="6" t="s">
         <v>78</v>
       </c>
@@ -4006,5 +4068,6 @@
     <mergeCell ref="A56:A57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>